<commit_message>
Checkers Remote two player
Adding Doug's updates for remote with repository connection
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>bdvals(cell#)</t>
   </si>
@@ -482,7 +482,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B3:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -580,7 +582,12 @@
       <c r="M5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="N5" s="2"/>
+      <c r="N5" s="2">
+        <v>5</v>
+      </c>
+      <c r="O5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="2:15" ht="22.5" customHeight="1">
       <c r="B6" s="6">
@@ -614,7 +621,7 @@
         <v>2</v>
       </c>
       <c r="N6" s="2">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="O6" t="s">
         <v>6</v>
@@ -652,7 +659,7 @@
         <v>3</v>
       </c>
       <c r="N7" s="2">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="O7" t="s">
         <v>6</v>
@@ -690,7 +697,7 @@
         <v>4</v>
       </c>
       <c r="N8" s="2">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="O8" t="s">
         <v>6</v>
@@ -728,7 +735,7 @@
         <v>5</v>
       </c>
       <c r="N9" s="2">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="O9" t="s">
         <v>6</v>

</xml_diff>